<commit_message>
Added more stuff. Most all is broken.
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>TC ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TCD ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>TR ID</t>
         </is>
       </c>
     </row>

</xml_diff>